<commit_message>
Update to ErrorSurface to normalize data
</commit_message>
<xml_diff>
--- a/PrelimResults.xlsx
+++ b/PrelimResults.xlsx
@@ -101,6 +101,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -122,6 +123,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -166,7 +168,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -176,10 +178,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -200,6 +198,7 @@
     <dxf>
       <font>
         <name val="Lohit Devanagari"/>
+        <charset val="1"/>
         <family val="2"/>
         <color rgb="FFFFFFFF"/>
       </font>
@@ -280,8 +279,8 @@
   </sheetPr>
   <dimension ref="A1:U203"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A184" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M206" activeCellId="0" sqref="M206"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A160" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="S183" activeCellId="0" sqref="S183"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2626,7 +2625,7 @@
         <v>4.27289843417</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="n">
         <v>35</v>
       </c>
@@ -13359,7 +13358,7 @@
         <f aca="false">SUM(B2:B201)/200</f>
         <v>8.68285073539091</v>
       </c>
-      <c r="C202" s="4" t="n">
+      <c r="C202" s="3" t="n">
         <f aca="false">SUM(C2:C201)/200</f>
         <v>41.0193255705796</v>
       </c>

</xml_diff>